<commit_message>
Formato a Fecha date-time. Armado de id de region.
Se modifica para que del dataframe se permita exportar la fecha en formato datetime adecuado para la Tabla MySql.
Se trabaja con archivos temporales para armar los códigos de las regiones.
</commit_message>
<xml_diff>
--- a/salida/regiones.xlsx
+++ b/salida/regiones.xlsx
@@ -443,413 +443,413 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> EL SURESTE DE AFGANISTáN </t>
+          <t xml:space="preserve"> NOROESTE DE LAS ISLAS KURILES </t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> YUNNAN, CHINA </t>
+          <t xml:space="preserve"> AL SUR DE LAS ISLAS FIJI </t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> CRETA, GRECIA </t>
+          <t xml:space="preserve"> ALASKA PENINSULA </t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> CERCA DE LA COSTA DE OREGON </t>
+          <t xml:space="preserve"> TIMOR REGIÓN </t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> SOUTHWEST OF SUMATRA, INDONESIA </t>
+          <t xml:space="preserve"> JÓNICO </t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> SOUTHWEST OF SUMATRA, INDONESIA </t>
+          <t xml:space="preserve"> NORTE DE ARGELIA </t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> SICHUAN, CHINA </t>
+          <t xml:space="preserve"> OESTE CHILE RISE </t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> SUR DE XINJIANG, CHINA </t>
+          <t xml:space="preserve"> CHILE-BOLIVIA FRONTERA REGIÓN </t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> AL SURESTE DE LAS ISLAS DE LEALTAD (LOYALTY) </t>
+          <t xml:space="preserve"> HOKKAIDO, JAPAN REGION </t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> MAR BANDA </t>
+          <t xml:space="preserve"> AL SUR DE LAS ISLAS FIJI </t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t xml:space="preserve"> CERCA LA COSTA ESTE DE KAMCHATKA </t>
+          <t xml:space="preserve"> NUEVA GUINEA, PAPUA NUEVA GUINEA </t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ISLAS KERMADAC, NUEVA ZELANDA </t>
+          <t xml:space="preserve"> CANAL DE LA MONA </t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ESTRECHO DE SUNDA, INDONESIA </t>
+          <t xml:space="preserve"> CENTRAL DE ITALIA </t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ISLAS SANTA CRUZ </t>
+          <t xml:space="preserve"> FLORES DEL MAR </t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t xml:space="preserve"> AL SUR DE LAS ISLAS KERMADAC </t>
+          <t xml:space="preserve"> REGIÓN DE LAS ISLAS SAMOA </t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t xml:space="preserve"> TAYIKISTÁN-XINJIANG REGIÓN FRONTERA </t>
+          <t xml:space="preserve"> KAZAJSTáN ORIENTAL </t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t xml:space="preserve"> SUR DE ALASKA </t>
+          <t xml:space="preserve"> CERCA DE COSTA DE NICARAGUA </t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ALASKA CENTRAL </t>
+          <t xml:space="preserve"> AFGANISTÁN-TAYIKISTÁN FRONT. REGIÓN </t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t xml:space="preserve"> HALMAHERA, INDONESIA </t>
+          <t xml:space="preserve"> TAIWÁN </t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t xml:space="preserve"> EN EL NORTE DE CHILE </t>
+          <t xml:space="preserve"> CERCA LA COSTA ESTE DE KAMCHATKA </t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t xml:space="preserve"> CERCA DE COSTA DE GUATEMALA </t>
+          <t xml:space="preserve"> ISLA NORTE, NUEVA ZELANDA </t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t xml:space="preserve"> CERCA LA COSTA E. DE HONSHU, JAPóN </t>
+          <t xml:space="preserve"> ISLAS SUR DE SANDWICH REGIÓN </t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t xml:space="preserve"> N DE LAS ISLAS ARU REGIÓ INDONESIA </t>
+          <t xml:space="preserve"> MAR BEAUFORT </t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t xml:space="preserve"> EL SUR DE IRáN </t>
+          <t xml:space="preserve"> ISLAS KURILES </t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t xml:space="preserve"> CERCA LA COSTA E. DE HONSHU, JAPóN </t>
+          <t xml:space="preserve"> JAVA, INDONESIA </t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ISLAS FIJI REGIÓN </t>
+          <t xml:space="preserve"> ISLAS SUR DE SANDWICH REGIÓN </t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t xml:space="preserve"> CANAL DE LA MONA </t>
+          <t xml:space="preserve"> CHILE-BOLIVIA FRONTERA REGIÓN </t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t xml:space="preserve"> AL SURESTE DE LAS ISLAS DE LEALTAD (LOYALTY) </t>
+          <t xml:space="preserve"> CERCA LA COSTA ESTE DE KAMCHATKA </t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t xml:space="preserve"> AL SUR DE LAS ISLAS FIJI </t>
+          <t xml:space="preserve"> SICHUAN, CHINA </t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PAKISTÁN </t>
+          <t xml:space="preserve"> BAFFIN REGIÓN DE LA ISLA, CANADA </t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t xml:space="preserve"> NORTE DE MAR DE LAS MOLUCAS </t>
+          <t xml:space="preserve"> ISLAS FIJI REGIÓN </t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t xml:space="preserve"> REGIÓN NUEVA IRLANDA, PNG </t>
+          <t xml:space="preserve"> ISLA DE ANDREANOF, ISLAS ALEUTIANAS </t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ISLAS SALOMÓN </t>
+          <t xml:space="preserve"> ISLAS KURILES </t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ECUADOR </t>
+          <t xml:space="preserve"> AFGANISTÁN-TAYIKISTÁN FRONT. REGIÓN </t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t xml:space="preserve"> EL NORTE DE XINJIANG, CHINA </t>
+          <t xml:space="preserve"> CERCA LA COSTA CENTRAL DE CHILE </t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t xml:space="preserve"> EN EL NORTE DE CHILE </t>
+          <t xml:space="preserve"> CHIPRE REGIóN </t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t xml:space="preserve"> CERCA LA COSTA E. DE HONSHU, JAPóN </t>
+          <t xml:space="preserve"> ESTE DEL LAGO BAIKAL, RUSIA </t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ISLAS SANTA CRUZ </t>
+          <t xml:space="preserve"> CERCA LA COSTA DE PERÚ </t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t xml:space="preserve"> EL OESTE DE TEXAS </t>
+          <t xml:space="preserve"> PANAMÁ-COSTA RICA REGIÓN FRONTERA </t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t xml:space="preserve"> EN EL NORTE DE CHILE </t>
+          <t xml:space="preserve"> CERCA LA COSTA CENTRAL DE CHILE </t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t xml:space="preserve"> EN EL NORTE DE INDIA </t>
+          <t xml:space="preserve"> CERCA LA COSTA CENTRAL DE CHILE </t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t xml:space="preserve"> REGIóN DE TAIWáN </t>
+          <t xml:space="preserve"> REGIÓN DE LAS ISLAS KERMADAC </t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t xml:space="preserve"> REGIóN DE TAIWáN </t>
+          <t xml:space="preserve"> LUZON, FILIPINAS </t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ISLAS FIJI REGIÓN </t>
+          <t xml:space="preserve"> ESTE MAR DE JAPÓN </t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t xml:space="preserve"> OAXACA, MÉXICO </t>
+          <t xml:space="preserve"> SUROESTE DE ÁFRICA </t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ISLAS FIJI REGIÓN </t>
+          <t xml:space="preserve"> ESTRECHO DE GIBRALTAR </t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t xml:space="preserve"> SUR DE PANAMÁ </t>
+          <t xml:space="preserve"> EL SURESTE DE AFGANISTáN </t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t xml:space="preserve"> SOUTHWEST OF SUMATRA, INDONESIA </t>
+          <t xml:space="preserve"> YUNNAN, CHINA </t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t xml:space="preserve"> E. RUSIA-NE CHINA FRONTERA REGIÓN </t>
+          <t xml:space="preserve"> CRETA, GRECIA </t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t xml:space="preserve"> SICHUAN, CHINA </t>
+          <t xml:space="preserve"> CERCA DE LA COSTA DE OREGON </t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t xml:space="preserve"> TAIWÁN </t>
+          <t xml:space="preserve"> SOUTHWEST OF SUMATRA, INDONESIA </t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t xml:space="preserve"> VOLCAN ISLAS, JAPÓN REGIÓN </t>
+          <t xml:space="preserve"> SOUTHWEST OF SUMATRA, INDONESIA </t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ISLAS SUR DE SANDWICH REGIÓN </t>
+          <t xml:space="preserve"> SICHUAN, CHINA </t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t xml:space="preserve"> EL SUR DE AUSTRALIA </t>
+          <t xml:space="preserve"> ISLAS VANUATU </t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t xml:space="preserve"> MINDANAO, FILIPINAS </t>
+          <t xml:space="preserve"> SUR DE XINJIANG, CHINA </t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t xml:space="preserve"> NUEVA BRETAÑA, PNG </t>
+          <t xml:space="preserve"> AL SURESTE DE LAS ISLAS DE LEALTAD (LOYALTY) </t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t xml:space="preserve"> OESTE DE LA ISLA MACQUARIE </t>
+          <t xml:space="preserve"> MAR BANDA </t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PENíNSULA DE KAMCHATKA, RUSIA </t>
+          <t xml:space="preserve"> CERCA LA COSTA ESTE DE KAMCHATKA </t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t xml:space="preserve"> CERCA LA COSTA CENTRAL DE CHILE </t>
+          <t xml:space="preserve"> ISLAS KERMADAC, NUEVA ZELANDA </t>
         </is>
       </c>
     </row>
@@ -863,280 +863,280 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t xml:space="preserve"> JAVA, INDONESIA </t>
+          <t xml:space="preserve"> ISLAS SANTA CRUZ </t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t xml:space="preserve"> MAR BANDA </t>
+          <t xml:space="preserve"> AL SUR DE LAS ISLAS KERMADAC </t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t xml:space="preserve"> FRENTE A LA COSTA DE CENTROAMÉRICA </t>
+          <t xml:space="preserve"> TAYIKISTÁN-XINJIANG REGIÓN FRONTERA </t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t xml:space="preserve"> EL SUR DE IRáN </t>
+          <t xml:space="preserve"> SUR DE ALASKA </t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PROVINCIA DE SAN JUAN, ARGENTINA </t>
+          <t xml:space="preserve"> ALASKA CENTRAL </t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t xml:space="preserve"> OESTE DE LA ISLA MACQUARIE </t>
+          <t xml:space="preserve"> HALMAHERA, INDONESIA </t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t xml:space="preserve"> REGIóN DE TAIWáN </t>
+          <t xml:space="preserve"> EN EL NORTE DE CHILE </t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t xml:space="preserve"> MINAHASSA PENINSULA, SULAWESI </t>
+          <t xml:space="preserve"> CERCA DE COSTA DE GUATEMALA </t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t xml:space="preserve"> MINDANAO, FILIPINAS </t>
+          <t xml:space="preserve"> CERCA LA COSTA E. DE HONSHU, JAPóN </t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t xml:space="preserve"> LUZON, FILIPINAS </t>
+          <t xml:space="preserve"> N DE LAS ISLAS ARU REGIÓ INDONESIA </t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t xml:space="preserve"> AL SUR DE LAS ISLAS MARIANA </t>
+          <t xml:space="preserve"> EL SUR DE IRáN </t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t xml:space="preserve"> MAR BANDA </t>
+          <t xml:space="preserve"> CERCA LA COSTA E. DE HONSHU, JAPóN </t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t xml:space="preserve"> KOMANDORSKIYE OSTROVA REGION </t>
+          <t xml:space="preserve"> ISLAS FIJI REGIÓN </t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t xml:space="preserve"> CERCA LA COSTA DE PERÚ </t>
+          <t xml:space="preserve"> CANAL DE LA MONA </t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t xml:space="preserve"> REGIóN DE TAIWáN </t>
+          <t xml:space="preserve"> AL SURESTE DE LAS ISLAS DE LEALTAD (LOYALTY) </t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t xml:space="preserve"> CERCA LA COSTA CENTRAL DE CHILE </t>
+          <t xml:space="preserve"> AL SUR DE LAS ISLAS FIJI </t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t xml:space="preserve"> VERACRUZ, MÉXICO </t>
+          <t xml:space="preserve"> PAKISTÁN </t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t xml:space="preserve"> RUSIA-MONGOLIA FRONTERA REGIÓN </t>
+          <t xml:space="preserve"> NORTE DE MAR DE LAS MOLUCAS </t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PROVINCIA DE SALTA, ARGENTINA </t>
+          <t xml:space="preserve"> REGIÓN NUEVA IRLANDA, PNG </t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t xml:space="preserve"> AL SUR DE LAS ISLAS FIJI </t>
+          <t xml:space="preserve"> ISLAS SALOMÓN </t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t xml:space="preserve"> REGIÓN DE LAS ISLAS TONGA </t>
+          <t xml:space="preserve"> ECUADOR </t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ISLAS SANTA CRUZ </t>
+          <t xml:space="preserve"> EL NORTE DE XINJIANG, CHINA </t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t xml:space="preserve"> NORTE DORSAL MEDIO-ATLANTICA </t>
+          <t xml:space="preserve"> EN EL NORTE DE CHILE </t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t xml:space="preserve"> NORTE DORSAL MEDIO-ATLANTICA </t>
+          <t xml:space="preserve"> CERCA LA COSTA E. DE HONSHU, JAPóN </t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t xml:space="preserve"> SUR DORSAL MEDIO-ATLANTICA </t>
+          <t xml:space="preserve"> ISLAS SANTA CRUZ </t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ISLA DE ANDREANOF, ISLAS ALEUTIANAS </t>
+          <t xml:space="preserve"> EL OESTE DE TEXAS </t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t xml:space="preserve"> REGIÓN DE LAS ISLAS TONGA </t>
+          <t xml:space="preserve"> EN EL NORTE DE CHILE </t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ISLAS FIJI REGIÓN </t>
+          <t xml:space="preserve"> EN EL NORTE DE INDIA </t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PACIFICO-ANTARTICO RIDGE </t>
+          <t xml:space="preserve"> REGIóN DE TAIWáN </t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ISLAS TONGA </t>
+          <t xml:space="preserve"> REGIóN DE TAIWáN </t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t xml:space="preserve"> CERCA LA COSTA OESTE DE HONSHU, JAPóN </t>
+          <t xml:space="preserve"> ISLAS FIJI REGIÓN </t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t xml:space="preserve"> AL SUR DE LAS ISLAS FIJI </t>
+          <t xml:space="preserve"> OAXACA, MÉXICO </t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t xml:space="preserve"> CERCA LA COSTA DE S. HONSHU, JAPóN </t>
+          <t xml:space="preserve"> ISLAS FIJI REGIÓN </t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t xml:space="preserve"> AFGANISTÁN-TAYIKISTÁN FRONT. REGIÓN </t>
+          <t xml:space="preserve"> SUR DE PANAMÁ </t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t xml:space="preserve"> AL SUR DE LAS ISLAS FIJI </t>
+          <t xml:space="preserve"> SOUTHWEST OF SUMATRA, INDONESIA </t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ISLAS BONIN, JAPON REGIÓN </t>
+          <t xml:space="preserve"> E. RUSIA-NE CHINA FRONTERA REGIÓN </t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t xml:space="preserve"> AL SUR DE LAS ISLAS FIJI </t>
+          <t xml:space="preserve"> SICHUAN, CHINA </t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t xml:space="preserve"> QINGHAI, CHINA </t>
+          <t xml:space="preserve"> TAIWÁN </t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t xml:space="preserve"> REYKJANES RIDGE </t>
+          <t xml:space="preserve"> VOLCAN ISLAS, JAPÓN REGIÓN </t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ESTE DE NEW GUINEA REG., PNG </t>
+          <t xml:space="preserve"> ISLAS SUR DE SANDWICH REGIÓN </t>
         </is>
       </c>
     </row>

</xml_diff>